<commit_message>
SQL INSERT and CREATE scripts up to date
</commit_message>
<xml_diff>
--- a/Tables/11.17 Updated Tables/Shuttle_11.15-1.xlsx
+++ b/Tables/11.17 Updated Tables/Shuttle_11.15-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/li-hsin/Desktop/MSBA Course/Final Project-Database/Raw Data/first version of excel tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aishwarya\Documents\GitHub\TERPcravingz\Tables\11.17 Updated Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B801C7B5-C4CC-1D4D-8C04-28EE7EF97B32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AE518D-38A4-4654-BB74-C76E5674BB9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B1727D5D-DE24-41C7-AC0E-AF0D1D25BF05}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B1727D5D-DE24-41C7-AC0E-AF0D1D25BF05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -647,13 +647,13 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -667,7 +667,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -681,7 +681,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>59</v>
       </c>
@@ -695,7 +695,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>60</v>
       </c>
@@ -709,7 +709,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>61</v>
       </c>
@@ -723,7 +723,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>62</v>
       </c>
@@ -737,7 +737,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>63</v>
       </c>
@@ -751,7 +751,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>64</v>
       </c>
@@ -765,7 +765,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>65</v>
       </c>
@@ -779,7 +779,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
@@ -793,7 +793,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>67</v>
       </c>
@@ -807,7 +807,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>68</v>
       </c>
@@ -821,7 +821,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>69</v>
       </c>
@@ -835,7 +835,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>70</v>
       </c>
@@ -849,7 +849,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
@@ -863,7 +863,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -877,7 +877,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>73</v>
       </c>
@@ -891,7 +891,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -905,7 +905,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -919,7 +919,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>76</v>
       </c>
@@ -933,7 +933,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>77</v>
       </c>
@@ -947,7 +947,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
@@ -961,7 +961,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>79</v>
       </c>
@@ -975,7 +975,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>80</v>
       </c>
@@ -989,7 +989,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>81</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>82</v>
       </c>

</xml_diff>